<commit_message>
:memo: add links in excel table
</commit_message>
<xml_diff>
--- a/documentos - tcc/planilha-controle-de-leitura_excel.xlsx
+++ b/documentos - tcc/planilha-controle-de-leitura_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iasmi\OneDrive\Documents\UFES\2024-2\TCC I\analise dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iasmi\OneDrive\Documents\UFES\2024-2\TCC I\dados - datasus [repositorio git]\srag_tcc\documentos - tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1CA09E-4474-4433-B648-BD8C38F4CD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4AEEFB-2A2C-4CB4-A92A-F0F34C997418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Relevância com relação a temática</t>
   </si>
@@ -170,33 +170,6 @@
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>Carlos A. Palacios, José A. Reyes-Suárez, Lorena A. Bearzotti , Víctor Leiva e Carolina Marchant</t>
-  </si>
-  <si>
-    <t>artigo</t>
-  </si>
-  <si>
-    <t>Descoberta de conhecimento para Retenção de estudantes do ensino superior baseado em mineração de dados: algoritmos de machine learning e estudo de casos no Chile</t>
-  </si>
-  <si>
-    <t>entropy-23-00485 (1).pdf</t>
-  </si>
-  <si>
-    <t>análise de dados; bancos de dados; ciência de dados; Teste de Friedman; explicacao de metodos</t>
-  </si>
-  <si>
-    <t>Semântica da Web: Ciência, Serviços e Agentes na rede mundial de computadores</t>
-  </si>
-  <si>
-    <t>Petar Ristoski∗, Heiko Paulheim</t>
-  </si>
-  <si>
-    <t>Dados abertos vinculados Web Semântica Mineração de dados</t>
-  </si>
-  <si>
-    <t>1-s2.0-S1570826816000020-main.en.pt.pdf</t>
   </si>
   <si>
     <t>https://rsdjournal.org/index.php/rsd/article/view/36173</t>
@@ -246,12 +219,64 @@
   <si>
     <t>https://repositorio.unesp.br/entities/publication/4f46fa86-57f0-45d5-aa0c-d3540da95bbf</t>
   </si>
+  <si>
+    <t>MODELO DE MACHINE LEARNING PARA PREDIÇÃO DE PROBLEMAS RESPIRATÓRIOS</t>
+  </si>
+  <si>
+    <t>Gustavo Torres Belini, Danilo da Silva Ataide e Johannes Von Lochter</t>
+  </si>
+  <si>
+    <t>Machine Learning, Síndrome Respiratória Aguda Grave, Modelos Preditivos, Gradient Boosting, Saúde Pública</t>
+  </si>
+  <si>
+    <t>https://www.ciaca-conf.org/wp-content/uploads/2024/12/CIACA2024_PT_F_021_Belini.pdf</t>
+  </si>
+  <si>
+    <t>06/052024</t>
+  </si>
+  <si>
+    <t>Vigilância em Saúde Pública; Sistemas de Informação em Saúde; Tomada de Decisões; Análise de Dados</t>
+  </si>
+  <si>
+    <t>Vanessa Coelho de Aquino Benjoino Ferraz
+Victor Vohryzek Ferezin
+Margarete Knoch
+Betina Durovni
+Valéria Saraceni
+Veruska Lahdo
+Mara Lisiane de Moraes dos Santos
+Alessandro Diogo De-Carli</t>
+  </si>
+  <si>
+    <t>Painéis de monitoramento de dados epidemiológicos como estratégia de gestão da vigilância e da atenção à saúde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1590/1413-812320242911.04142024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bdtd.ucb.br:8443/jspui/handle/tede/3198#preview-link0 </t>
+  </si>
+  <si>
+    <t>Machine Learning e Análise Preditiva em saúde: um
+estudo de caso sobre detecção de anomalias em contas
+médicas do Exército</t>
+  </si>
+  <si>
+    <t>Dissertação</t>
+  </si>
+  <si>
+    <t>Sergio Ricardo Pacheco da Vitoria</t>
+  </si>
+  <si>
+    <t>DBSCAN; ISOLATION FOREST; contas médicas; SAMMED;
+auditoria; Machine Learnng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -307,20 +332,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF646464"/>
       <name val="Arial"/>
@@ -364,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -465,12 +476,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -499,34 +523,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -536,17 +547,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -863,25 +892,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:W996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" style="17" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17" style="24" customWidth="1"/>
-    <col min="6" max="6" width="85.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17" style="17" customWidth="1"/>
+    <col min="6" max="6" width="85.88671875" style="17" customWidth="1"/>
     <col min="7" max="23" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -910,7 +939,7 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="14.4">
-      <c r="A2" s="25"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -937,7 +966,7 @@
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" ht="14.4">
-      <c r="A3" s="26"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1000,24 +1029,24 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" s="24" customFormat="1" ht="79.2">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:23" ht="66.599999999999994">
+      <c r="A5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="13">
+        <v>44877</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="F5" s="26" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="15">
-        <v>44306</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>13</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1037,23 +1066,23 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" ht="66.599999999999994">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:23" ht="66">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>11</v>
+      <c r="B6" s="12" t="s">
+        <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="15">
-        <v>42370</v>
+      <c r="D6" s="13">
+        <v>44440</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>17</v>
+      <c r="E6" s="12" t="s">
+        <v>19</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="3"/>
@@ -1074,13 +1103,25 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" ht="14.4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="13"/>
+    <row r="7" spans="1:23" ht="118.8">
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="13">
+        <v>44403</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1099,13 +1140,23 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" ht="14.4">
-      <c r="A8" s="22"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="13"/>
+    <row r="8" spans="1:23" ht="39" customHeight="1">
+      <c r="A8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1124,24 +1175,24 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" ht="66.599999999999994">
-      <c r="A9" s="22" t="s">
-        <v>22</v>
+    <row r="9" spans="1:23" ht="119.4">
+      <c r="A9" s="20" t="s">
+        <v>32</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>21</v>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>23</v>
+      <c r="C9" s="15" t="s">
+        <v>31</v>
       </c>
-      <c r="D9" s="15">
-        <v>44877</v>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>20</v>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>19</v>
+      <c r="F9" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1161,24 +1212,24 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" ht="52.8">
-      <c r="A10" s="14" t="s">
-        <v>24</v>
+    <row r="10" spans="1:23" ht="93">
+      <c r="A10" s="15" t="s">
+        <v>35</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
+      <c r="B10" s="12" t="s">
+        <v>36</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>25</v>
+      <c r="C10" s="15" t="s">
+        <v>37</v>
       </c>
-      <c r="D10" s="15">
-        <v>44440</v>
+      <c r="D10" s="13">
+        <v>44624</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>28</v>
+      <c r="E10" s="15" t="s">
+        <v>38</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>27</v>
+      <c r="F10" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1198,25 +1249,13 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" ht="118.8">
-      <c r="A11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="15">
-        <v>44403</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>33</v>
-      </c>
+    <row r="11" spans="1:23" ht="60.6" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1235,13 +1274,13 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:23" ht="39" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="17"/>
+    <row r="12" spans="1:23" ht="14.4">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1261,12 +1300,12 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="14.4">
-      <c r="A13" s="22"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1286,12 +1325,12 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="14.4">
-      <c r="A14" s="22"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1310,13 +1349,13 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" ht="60.6" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="19"/>
+    <row r="15" spans="1:23" ht="14.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1336,12 +1375,12 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="14.4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1360,13 +1399,13 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" ht="14.4">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1385,13 +1424,13 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" ht="14.4">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1410,13 +1449,13 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" ht="14.4">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1435,7 +1474,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" ht="14.4">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1460,7 +1499,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1">
+    <row r="21" spans="1:23" ht="41.25" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1490,8 +1529,8 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1516,7 +1555,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1560,7 +1599,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" ht="41.25" customHeight="1">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1611,12 +1650,12 @@
       <c r="W26" s="3"/>
     </row>
     <row r="27" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1636,12 +1675,12 @@
       <c r="W27" s="3"/>
     </row>
     <row r="28" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1661,12 +1700,12 @@
       <c r="W28" s="3"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1686,12 +1725,12 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1711,12 +1750,12 @@
       <c r="W30" s="3"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -1736,12 +1775,12 @@
       <c r="W31" s="3"/>
     </row>
     <row r="32" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -25860,117 +25899,21 @@
       <c r="V996" s="3"/>
       <c r="W996" s="3"/>
     </row>
-    <row r="997" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A997" s="3"/>
-      <c r="B997" s="3"/>
-      <c r="C997" s="3"/>
-      <c r="D997" s="3"/>
-      <c r="E997" s="3"/>
-      <c r="F997" s="3"/>
-      <c r="G997" s="3"/>
-      <c r="H997" s="3"/>
-      <c r="I997" s="3"/>
-      <c r="J997" s="3"/>
-      <c r="K997" s="3"/>
-      <c r="L997" s="3"/>
-      <c r="M997" s="3"/>
-      <c r="N997" s="3"/>
-      <c r="O997" s="3"/>
-      <c r="P997" s="3"/>
-      <c r="Q997" s="3"/>
-      <c r="R997" s="3"/>
-      <c r="S997" s="3"/>
-      <c r="T997" s="3"/>
-      <c r="U997" s="3"/>
-      <c r="V997" s="3"/>
-      <c r="W997" s="3"/>
-    </row>
-    <row r="998" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A998" s="3"/>
-      <c r="B998" s="3"/>
-      <c r="C998" s="3"/>
-      <c r="D998" s="3"/>
-      <c r="E998" s="3"/>
-      <c r="F998" s="3"/>
-      <c r="G998" s="3"/>
-      <c r="H998" s="3"/>
-      <c r="I998" s="3"/>
-      <c r="J998" s="3"/>
-      <c r="K998" s="3"/>
-      <c r="L998" s="3"/>
-      <c r="M998" s="3"/>
-      <c r="N998" s="3"/>
-      <c r="O998" s="3"/>
-      <c r="P998" s="3"/>
-      <c r="Q998" s="3"/>
-      <c r="R998" s="3"/>
-      <c r="S998" s="3"/>
-      <c r="T998" s="3"/>
-      <c r="U998" s="3"/>
-      <c r="V998" s="3"/>
-      <c r="W998" s="3"/>
-    </row>
-    <row r="999" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A999" s="3"/>
-      <c r="B999" s="3"/>
-      <c r="C999" s="3"/>
-      <c r="D999" s="3"/>
-      <c r="E999" s="3"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="3"/>
-      <c r="J999" s="3"/>
-      <c r="K999" s="3"/>
-      <c r="L999" s="3"/>
-      <c r="M999" s="3"/>
-      <c r="N999" s="3"/>
-      <c r="O999" s="3"/>
-      <c r="P999" s="3"/>
-      <c r="Q999" s="3"/>
-      <c r="R999" s="3"/>
-      <c r="S999" s="3"/>
-      <c r="T999" s="3"/>
-      <c r="U999" s="3"/>
-      <c r="V999" s="3"/>
-      <c r="W999" s="3"/>
-    </row>
-    <row r="1000" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="3"/>
-      <c r="J1000" s="3"/>
-      <c r="K1000" s="3"/>
-      <c r="L1000" s="3"/>
-      <c r="M1000" s="3"/>
-      <c r="N1000" s="3"/>
-      <c r="O1000" s="3"/>
-      <c r="P1000" s="3"/>
-      <c r="Q1000" s="3"/>
-      <c r="R1000" s="3"/>
-      <c r="S1000" s="3"/>
-      <c r="T1000" s="3"/>
-      <c r="U1000" s="3"/>
-      <c r="V1000" s="3"/>
-      <c r="W1000" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{52C6E326-F294-438D-849B-8BAC8BD31FAC}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{29204FDA-71AF-4EFA-A662-4CDDCE5F63CE}"/>
-    <hyperlink ref="F11" r:id="rId3" xr:uid="{40F53EF2-BE3C-4073-A90F-E9BE43736A59}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{52C6E326-F294-438D-849B-8BAC8BD31FAC}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{29204FDA-71AF-4EFA-A662-4CDDCE5F63CE}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{40F53EF2-BE3C-4073-A90F-E9BE43736A59}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{FF76384E-DBBA-4216-894E-18DB78027B9C}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{56463920-380D-4D6D-B33F-0E50F5F2645F}"/>
+    <hyperlink ref="A9" r:id="rId6" display="https://www.scielosp.org/article/csc/2024.v29n11/e04142024/pt/" xr:uid="{476A888D-8D85-4EB3-B431-FB8D162C1F9B}"/>
+    <hyperlink ref="F10" r:id="rId7" location="preview-link0 " xr:uid="{F6970C39-ABDF-42D5-9FEF-5E64FB0880A4}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:page_facing_up: add new links in excel table
</commit_message>
<xml_diff>
--- a/documentos - tcc/planilha-controle-de-leitura_excel.xlsx
+++ b/documentos - tcc/planilha-controle-de-leitura_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iasmi\OneDrive\Documents\UFES\2024-2\TCC I\dados - datasus [repositorio git]\srag_tcc\documentos - tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4AEEFB-2A2C-4CB4-A92A-F0F34C997418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C02A4-E562-48D0-88A8-DD3807DBA237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Relevância com relação a temática</t>
   </si>
@@ -271,12 +271,27 @@
     <t>DBSCAN; ISOLATION FOREST; contas médicas; SAMMED;
 auditoria; Machine Learnng</t>
   </si>
+  <si>
+    <t>Covid-19; Sars-CoV-2; Modelos logísticos; Inteligência artificial; Aprendizado de máquina</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1590/0103-11042022E809</t>
+  </si>
+  <si>
+    <t>Risomario ilva, Darcy Ramos da ilva Neto</t>
+  </si>
+  <si>
+    <t>Inteligência artificial e previsão de óbito por
+Covid-19 no Brasil: uma análise comparativa
+entre os algoritmos Logistic Regression,
+Decision Tree e Random Forest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -340,6 +355,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -464,19 +486,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -489,12 +498,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -556,6 +580,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,17 +598,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -894,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -910,7 +937,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -939,7 +966,7 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="14.4">
-      <c r="A2" s="22"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -966,7 +993,7 @@
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" ht="14.4">
-      <c r="A3" s="23"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1029,7 +1056,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" ht="66.599999999999994">
+    <row r="5" spans="1:23" ht="84.6" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
@@ -1045,7 +1072,7 @@
       <c r="E5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="3"/>
@@ -1082,7 +1109,7 @@
       <c r="E6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="22" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="3"/>
@@ -1141,7 +1168,7 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:23" ht="39" customHeight="1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1191,7 +1218,7 @@
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="3"/>
@@ -1228,7 +1255,7 @@
       <c r="E10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="22" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="3"/>
@@ -1249,13 +1276,25 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" ht="60.6" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="25"/>
+    <row r="11" spans="1:23" ht="100.8">
+      <c r="A11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="13">
+        <v>44858</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1275,7 +1314,7 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="14.4">
-      <c r="A12" s="11"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1330,7 +1369,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="27"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1455,7 +1494,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -25911,9 +25950,11 @@
     <hyperlink ref="F9" r:id="rId5" xr:uid="{56463920-380D-4D6D-B33F-0E50F5F2645F}"/>
     <hyperlink ref="A9" r:id="rId6" display="https://www.scielosp.org/article/csc/2024.v29n11/e04142024/pt/" xr:uid="{476A888D-8D85-4EB3-B431-FB8D162C1F9B}"/>
     <hyperlink ref="F10" r:id="rId7" location="preview-link0 " xr:uid="{F6970C39-ABDF-42D5-9FEF-5E64FB0880A4}"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://www.scielosp.org/article/sdeb/2022.v46nspe8/118-129/pt/" xr:uid="{28181F7E-1D9B-45AC-ACA0-9D1E8E5F5461}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{52DDC651-910C-4DEA-9B2E-52D762DEDB2F}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>